<commit_message>
[LC-850] Release of LetsCo OS v1.3.0
Signed-off-by: OUESLATI Wyem Ext <wyem.oueslati@rte-france.com>
</commit_message>
<xml_diff>
--- a/_site/documentation/asciidoc/implementation_guide/attached_doc/excel_header_input_file.xlsx
+++ b/_site/documentation/asciidoc/implementation_guide/attached_doc/excel_header_input_file.xlsx
@@ -221,7 +221,7 @@
     <t xml:space="preserve">rscKpi</t>
   </si>
   <si>
-    <t xml:space="preserve">GP1</t>
+    <t xml:space="preserve">GP01</t>
   </si>
   <si>
     <t xml:space="preserve">ProcessSuccess</t>
@@ -233,7 +233,7 @@
     <t xml:space="preserve">2020-03-18T01:00:00Z</t>
   </si>
   <si>
-    <t xml:space="preserve">GP2</t>
+    <t xml:space="preserve">GP02</t>
   </si>
   <si>
     <t xml:space="preserve">CalculationFailed</t>
@@ -245,7 +245,7 @@
     <t xml:space="preserve">Y</t>
   </si>
   <si>
-    <t xml:space="preserve">GP3</t>
+    <t xml:space="preserve">GP03</t>
   </si>
   <si>
     <t xml:space="preserve">ProcessDelayed</t>
@@ -254,7 +254,7 @@
     <t xml:space="preserve">DelayTime</t>
   </si>
   <si>
-    <t xml:space="preserve">BP1</t>
+    <t xml:space="preserve">BP01</t>
   </si>
   <si>
     <t xml:space="preserve">BusinessKpiAServiceA</t>
@@ -275,13 +275,13 @@
     <t xml:space="preserve">34X-0000000068-Q</t>
   </si>
   <si>
-    <t xml:space="preserve">BP2</t>
+    <t xml:space="preserve">BP02</t>
   </si>
   <si>
     <t xml:space="preserve">BusinessKpiBServiceA</t>
   </si>
   <si>
-    <t xml:space="preserve">BP3</t>
+    <t xml:space="preserve">BP03</t>
   </si>
   <si>
     <t xml:space="preserve">BusinessKpiCServiceA</t>
@@ -1077,10 +1077,10 @@
   </sheetPr>
   <dimension ref="A1:U288"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>